<commit_message>
Added pages in framework and updated TC accordingly
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Master_Sheet.xlsx
+++ b/src/test/resources/testData/Master_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BYMAT-Learn_Automation\WorkSpace\WorkSpace_Photon\SeleniumTraining_B10_MVN\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A26ACF-A50B-44A3-B512-489A5D5F1552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C14DB01-C889-4427-A35C-A9B03BC0B120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
@@ -19,14 +19,14 @@
   </sheets>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
+    <customWorkbookView name="Ganjare, Rahul - Personal View" guid="{2F07CA58-5A36-422D-B734-0409EAA0C515}" mergeInterval="0" personalView="1" maximized="1" xWindow="-11" yWindow="-11" windowWidth="1942" windowHeight="1042" activeSheetId="3"/>
     <customWorkbookView name="admin - Personal View" guid="{17DC0733-3E6C-4403-A6F2-366590E0F695}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="542" activeSheetId="2"/>
-    <customWorkbookView name="Ganjare, Rahul - Personal View" guid="{2F07CA58-5A36-422D-B734-0409EAA0C515}" mergeInterval="0" personalView="1" maximized="1" xWindow="-11" yWindow="-11" windowWidth="1942" windowHeight="1042" activeSheetId="3"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="46">
   <si>
     <t>Sr.No</t>
   </si>
@@ -155,6 +155,15 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>EndToEndTestCase</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>EndToEnd</t>
   </si>
 </sst>
 </file>
@@ -206,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -229,12 +238,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -248,6 +268,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -589,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A241FC5-44F1-4997-99CE-4E28269E2CD0}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -654,7 +680,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -666,6 +692,17 @@
       </c>
       <c r="C6" s="7" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -681,10 +718,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91A57E9-F358-48D5-93F4-31EDBA8F47AC}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1053,6 +1090,70 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="6">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -1060,6 +1161,7 @@
     <hyperlink ref="E11" r:id="rId2" xr:uid="{989E40D4-E156-4F76-9CBC-6900BEA8358B}"/>
     <hyperlink ref="E15" r:id="rId3" xr:uid="{035103AE-818F-400C-BF4A-295F6ECC6D8D}"/>
     <hyperlink ref="E19" r:id="rId4" xr:uid="{6B2447C9-2ACC-46A8-86BC-D9B0E02B292A}"/>
+    <hyperlink ref="E23" r:id="rId5" xr:uid="{3761A8D2-5A39-484B-B4AD-2980CEED10AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>